<commit_message>
Updated Excel and readme with contributions
</commit_message>
<xml_diff>
--- a/SOEN287A2Grading (1).xlsx
+++ b/SOEN287A2Grading (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GhaithAdnan\Documents\GitHub\SOEN-287\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamo\Documents\GitHub\SOEN-287\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D457F07-290F-4F58-8FC5-941731B8A338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8972558-4799-4C08-A20B-A1F33BE28195}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Grading Sheet for SOEN 287/Winter 2021</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Ghaith Chrit 40114180</t>
+  </si>
+  <si>
+    <t>Adamo Orsini 40174716</t>
   </si>
 </sst>
 </file>
@@ -548,14 +551,27 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -563,23 +579,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -812,18 +815,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
     </row>
     <row r="3" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -852,11 +855,11 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="41" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="28" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="8"/>
@@ -872,11 +875,11 @@
       <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="41" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="28" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="13"/>
@@ -892,10 +895,10 @@
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="31"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="14" t="s">
         <v>13</v>
       </c>
@@ -936,10 +939,10 @@
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="31"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="14" t="s">
         <v>13</v>
       </c>
@@ -956,11 +959,13 @@
       <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -974,11 +979,13 @@
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -992,10 +999,10 @@
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="31"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="16"/>
       <c r="E18" s="13"/>
     </row>
@@ -1010,10 +1017,10 @@
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="31"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="7"/>
       <c r="E20" s="13"/>
     </row>
@@ -1028,10 +1035,10 @@
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="31"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="7"/>
       <c r="E22" s="13"/>
     </row>
@@ -1046,10 +1053,10 @@
       <c r="E23" s="12"/>
     </row>
     <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="31"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="7"/>
       <c r="E24" s="13"/>
     </row>
@@ -1064,10 +1071,10 @@
       <c r="E25" s="12"/>
     </row>
     <row r="26" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="31"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="7"/>
       <c r="E26" s="13"/>
     </row>
@@ -1082,10 +1089,10 @@
       <c r="E27" s="12"/>
     </row>
     <row r="28" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="31"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="7"/>
       <c r="E28" s="13"/>
     </row>
@@ -1100,10 +1107,10 @@
       <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="31"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="7"/>
       <c r="E30" s="4"/>
     </row>
@@ -1117,11 +1124,11 @@
       <c r="C31" s="20"/>
     </row>
     <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="30"/>
     </row>
     <row r="33" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
@@ -1144,18 +1151,18 @@
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="31"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="4"/>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="31"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="23"/>
     </row>
     <row r="37" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1168,17 +1175,17 @@
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="37"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="39"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="23"/>
     </row>
     <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1191,10 +1198,10 @@
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="30"/>
     </row>
     <row r="42" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2157,6 +2164,16 @@
     <row r="1000" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
@@ -2168,16 +2185,6 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>